<commit_message>
feat: drop row nan
</commit_message>
<xml_diff>
--- a/data_range_report/JP - Date Range Report - duffyh318@gmail.com.xlsx
+++ b/data_range_report/JP - Date Range Report - duffyh318@gmail.com.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.9.10\NAS - AMZ - Sales - 01\AMZ - Customer Support\File Báo Cáo\Báo Cáo Tháng\11.2021\JP\duffyh318@gmail.com\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\iart_data_port_upload\data_range_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482F1D33-993B-4335-BE4B-3B7C236A77BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8202719-584E-445B-A81C-81B11429BDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="14970" windowHeight="10485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="duffyh318@gmail.com" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t xml:space="preserve">Amazon o•iƒT[ƒrƒXAƒtƒ‹ƒtƒBƒ‹ƒƒ“ƒg by Amazon (FBA) </t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>ƒvƒƒ‚[ƒVƒ‡ƒ“Š„ˆø‚ÌÅ‹à</t>
-  </si>
-  <si>
-    <t>Œ¹ò’¥ŽûÅ‚ð”º‚¤ƒ}[ƒPƒbƒgƒvƒŒƒCƒX</t>
   </si>
   <si>
     <t>Žè”—¿</t>
@@ -700,9 +697,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -740,7 +737,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -846,7 +843,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -988,7 +985,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -999,7 +996,7 @@
   <dimension ref="A1:AB11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,40 +1103,37 @@
       <c r="V8" t="s">
         <v>28</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>29</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>30</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>31</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>32</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>33</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9">
         <v>10987108593</v>
       </c>
       <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" t="s">
         <v>36</v>
-      </c>
-      <c r="F9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" t="s">
-        <v>37</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -1189,19 +1183,19 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10">
         <v>10987108593</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -1251,16 +1245,16 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11">
         <v>11006283493</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N11">
         <v>0</v>

</xml_diff>